<commit_message>
Finishing up the couple of things missing? Let's be optimistic
</commit_message>
<xml_diff>
--- a/output/sites/test_differences_nut_all_scenarios_Pointe Suzanne.xlsx
+++ b/output/sites/test_differences_nut_all_scenarios_Pointe Suzanne.xlsx
@@ -475,22 +475,22 @@
         <v>11</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.009</v>
       </c>
       <c r="E3" t="n">
-        <v>0.157</v>
+        <v>0.225</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G3" t="n">
-        <v>0.002</v>
+        <v>0.006</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="4">
@@ -504,22 +504,22 @@
         <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.182</v>
       </c>
       <c r="E4" t="n">
-        <v>0.194</v>
+        <v>0.395</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.154</v>
       </c>
       <c r="G4" t="n">
-        <v>0.004</v>
+        <v>0.202</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.111</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>0.192</v>
       </c>
     </row>
     <row r="5">
@@ -533,22 +533,22 @@
         <v>13</v>
       </c>
       <c r="D5" t="n">
-        <v>0.013</v>
+        <v>0.81</v>
       </c>
       <c r="E5" t="n">
-        <v>0.259</v>
+        <v>0.591</v>
       </c>
       <c r="F5" t="n">
-        <v>0.006</v>
+        <v>0.842</v>
       </c>
       <c r="G5" t="n">
-        <v>0.022</v>
+        <v>0.814</v>
       </c>
       <c r="H5" t="n">
-        <v>0.003</v>
+        <v>0.87</v>
       </c>
       <c r="I5" t="n">
-        <v>0.011</v>
+        <v>0.812</v>
       </c>
     </row>
     <row r="6">
@@ -562,22 +562,22 @@
         <v>14</v>
       </c>
       <c r="D6" t="n">
-        <v>0.107</v>
+        <v>0.998</v>
       </c>
       <c r="E6" t="n">
-        <v>0.364</v>
+        <v>0.777</v>
       </c>
       <c r="F6" t="n">
-        <v>0.073</v>
+        <v>0.999</v>
       </c>
       <c r="G6" t="n">
-        <v>0.131</v>
+        <v>0.996</v>
       </c>
       <c r="H6" t="n">
-        <v>0.051</v>
+        <v>0.999</v>
       </c>
       <c r="I6" t="n">
-        <v>0.111</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="7">
@@ -591,22 +591,22 @@
         <v>15</v>
       </c>
       <c r="D7" t="n">
-        <v>0.477</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.478</v>
+        <v>0.908</v>
       </c>
       <c r="F7" t="n">
-        <v>0.481</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>0.488</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.472</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>0.483</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -620,22 +620,22 @@
         <v>16</v>
       </c>
       <c r="D8" t="n">
-        <v>0.929</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0.66</v>
+        <v>0.972</v>
       </c>
       <c r="F8" t="n">
-        <v>0.963</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>0.916</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>0.976</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.937</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -649,22 +649,22 @@
         <v>17</v>
       </c>
       <c r="D9" t="n">
-        <v>0.999</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.843</v>
+        <v>0.995</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>0.999</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0.999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -681,7 +681,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.951</v>
+        <v>0.999</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -710,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0.999</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
@@ -823,22 +823,22 @@
         <v>12</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0.978</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0.809</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>0.955</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0.977</v>
       </c>
     </row>
     <row r="16">
@@ -852,22 +852,22 @@
         <v>13</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0.044</v>
       </c>
       <c r="E16" t="n">
-        <v>0.995</v>
+        <v>0.188</v>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>0.079</v>
       </c>
       <c r="G16" t="n">
-        <v>1</v>
+        <v>0.059</v>
       </c>
       <c r="H16" t="n">
-        <v>1</v>
+        <v>0.121</v>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0.041</v>
       </c>
     </row>
     <row r="17">
@@ -881,22 +881,22 @@
         <v>14</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.898</v>
+        <v>0.014</v>
       </c>
       <c r="F17" t="n">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0.996</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>0.978</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>0.998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -910,22 +910,22 @@
         <v>15</v>
       </c>
       <c r="D18" t="n">
-        <v>0.481</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0.488</v>
+        <v>0.001</v>
       </c>
       <c r="F18" t="n">
-        <v>0.479</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.49</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0.484</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>0.478</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -939,22 +939,22 @@
         <v>16</v>
       </c>
       <c r="D19" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.086</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0.003</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0.023</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1113,19 +1113,19 @@
         <v>11</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="E25" t="n">
-        <v>0.005</v>
+        <v>0.028</v>
       </c>
       <c r="F25" t="n">
-        <v>0.014</v>
+        <v>0.056</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="H25" t="n">
-        <v>0.311</v>
+        <v>0.365</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
@@ -1142,22 +1142,22 @@
         <v>12</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>0.167</v>
       </c>
       <c r="E26" t="n">
-        <v>0.022</v>
+        <v>0.291</v>
       </c>
       <c r="F26" t="n">
-        <v>0.029</v>
+        <v>0.296</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>0.177</v>
       </c>
       <c r="H26" t="n">
-        <v>0.346</v>
+        <v>0.44</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>0.169</v>
       </c>
     </row>
     <row r="27">
@@ -1171,22 +1171,22 @@
         <v>13</v>
       </c>
       <c r="D27" t="n">
-        <v>0.005</v>
+        <v>0.81</v>
       </c>
       <c r="E27" t="n">
-        <v>0.072</v>
+        <v>0.716</v>
       </c>
       <c r="F27" t="n">
-        <v>0.091</v>
+        <v>0.694</v>
       </c>
       <c r="G27" t="n">
-        <v>0.011</v>
+        <v>0.817</v>
       </c>
       <c r="H27" t="n">
-        <v>0.39</v>
+        <v>0.532</v>
       </c>
       <c r="I27" t="n">
-        <v>0.009</v>
+        <v>0.818</v>
       </c>
     </row>
     <row r="28">
@@ -1200,22 +1200,22 @@
         <v>14</v>
       </c>
       <c r="D28" t="n">
-        <v>0.103</v>
+        <v>0.994</v>
       </c>
       <c r="E28" t="n">
-        <v>0.183</v>
+        <v>0.96</v>
       </c>
       <c r="F28" t="n">
-        <v>0.226</v>
+        <v>0.953</v>
       </c>
       <c r="G28" t="n">
-        <v>0.105</v>
+        <v>0.997</v>
       </c>
       <c r="H28" t="n">
-        <v>0.443</v>
+        <v>0.603</v>
       </c>
       <c r="I28" t="n">
-        <v>0.095</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="29">
@@ -1229,22 +1229,22 @@
         <v>15</v>
       </c>
       <c r="D29" t="n">
-        <v>0.478</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>0.498</v>
+        <v>0.999</v>
       </c>
       <c r="F29" t="n">
-        <v>0.482</v>
+        <v>0.996</v>
       </c>
       <c r="G29" t="n">
-        <v>0.472</v>
+        <v>1</v>
       </c>
       <c r="H29" t="n">
-        <v>0.481</v>
+        <v>0.689</v>
       </c>
       <c r="I29" t="n">
-        <v>0.46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1258,22 +1258,22 @@
         <v>16</v>
       </c>
       <c r="D30" t="n">
-        <v>0.938</v>
+        <v>1</v>
       </c>
       <c r="E30" t="n">
-        <v>0.834</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
-        <v>0.807</v>
+        <v>1</v>
       </c>
       <c r="G30" t="n">
-        <v>0.938</v>
+        <v>1</v>
       </c>
       <c r="H30" t="n">
-        <v>0.567</v>
+        <v>0.781</v>
       </c>
       <c r="I30" t="n">
-        <v>0.939</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1287,22 +1287,22 @@
         <v>17</v>
       </c>
       <c r="D31" t="n">
-        <v>0.998</v>
+        <v>1</v>
       </c>
       <c r="E31" t="n">
-        <v>0.986</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
-        <v>0.974</v>
+        <v>1</v>
       </c>
       <c r="G31" t="n">
-        <v>0.996</v>
+        <v>1</v>
       </c>
       <c r="H31" t="n">
-        <v>0.651</v>
+        <v>0.838</v>
       </c>
       <c r="I31" t="n">
-        <v>0.998</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1328,7 +1328,7 @@
         <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>0.751</v>
+        <v>0.88</v>
       </c>
       <c r="I32" t="n">
         <v>1</v>
@@ -1357,7 +1357,7 @@
         <v>1</v>
       </c>
       <c r="H33" t="n">
-        <v>0.856</v>
+        <v>0.919</v>
       </c>
       <c r="I33" t="n">
         <v>1</v>

</xml_diff>